<commit_message>
[Shashi] corrected transaction total amount calculation
</commit_message>
<xml_diff>
--- a/docs/Test_case.xlsx
+++ b/docs/Test_case.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28695" windowHeight="12780"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Place</t>
   </si>
@@ -27,21 +27,9 @@
     <t>Details</t>
   </si>
   <si>
-    <t>The first item selected doesn’t display item price</t>
-  </si>
-  <si>
-    <t>Restrictions</t>
-  </si>
-  <si>
-    <t>This happens only for the first item</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
-    <t>Very high</t>
-  </si>
-  <si>
     <t>Item screen</t>
   </si>
   <si>
@@ -79,6 +67,40 @@
   </si>
   <si>
     <t>replace characters by descriptions</t>
+  </si>
+  <si>
+    <t>Procurement Transaction</t>
+  </si>
+  <si>
+    <t>Very High</t>
+  </si>
+  <si>
+    <t>Transaction header also has the same wrong amount - table procurement_transaction</t>
+  </si>
+  <si>
+    <t>The first item selected doesn’t display item price. This happens only for the first item</t>
+  </si>
+  <si>
+    <t>Transaction type should be changed to type P not S - P sound more intuitive.</t>
+  </si>
+  <si>
+    <t>Save a Pt and then using new transaction - the item price not updated - sporadic</t>
+  </si>
+  <si>
+    <t>After transaction is saved - the resulting screen header says Vendor details</t>
+  </si>
+  <si>
+    <t>format date and type of transaction after save transaction.</t>
+  </si>
+  <si>
+    <t>Transaction Details</t>
+  </si>
+  <si>
+    <t>Fetch transactions not working</t>
+  </si>
+  <si>
+    <t>Item details amount calculated and stored is not
+ total amount but price/per item - PtDetails table</t>
   </si>
 </sst>
 </file>
@@ -114,8 +136,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,20 +435,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="71.140625" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,91 +455,168 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>